<commit_message>
Improve generator with random strings, add parametrization to add group test
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olegi\PycharmProjects\python_win_gui\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{773413DA-758E-4C59-9EB6-52EC11A72DD2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94F88730-409B-48CE-81BA-712EEF86DD41}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6564" xr2:uid="{69EF5D49-239B-48F6-9575-1170ED5EC1C7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6564" xr2:uid="{7D4E1158-4F9E-44EC-BD21-B23D09E6B3F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,36 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>group0</t>
+    <t>g2844</t>
   </si>
   <si>
-    <t>group1</t>
+    <t>g4zUdx</t>
   </si>
   <si>
-    <t>group2</t>
+    <t>g</t>
   </si>
   <si>
-    <t>group3</t>
+    <t>gGzap</t>
   </si>
   <si>
-    <t>group4</t>
-  </si>
-  <si>
-    <t>group5</t>
-  </si>
-  <si>
-    <t>group6</t>
-  </si>
-  <si>
-    <t>group7</t>
-  </si>
-  <si>
-    <t>group8</t>
-  </si>
-  <si>
-    <t>group9</t>
+    <t>g 3p</t>
   </si>
 </sst>
 </file>
@@ -406,8 +391,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFFC562-6F77-4D21-8228-FB3743B98E0A}">
-  <dimension ref="A1:A10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85403BCB-4DBC-495B-9AC5-2DF87131C439}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -438,31 +423,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>